<commit_message>
Cleaner code with two different model versions (with repeatvector and without)
</commit_message>
<xml_diff>
--- a/src/models/Model_stats.xlsx
+++ b/src/models/Model_stats.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mf/Desktop/CS/Studies/7_Final_Project/Kaggle_M5PointPrediction/src/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EDE6BC-EDB8-1345-AC79-3939BD99D428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711B639E-C4B8-8548-9CF0-487A90B0278E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C69EC06E-22E8-864B-AAEF-80B6061A84A1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{C69EC06E-22E8-864B-AAEF-80B6061A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -131,10 +131,10 @@
     <t>Original model</t>
   </si>
   <si>
-    <t>30,490; 7; 20?</t>
-  </si>
-  <si>
-    <t>30,490 batches per each run</t>
+    <t>1941 times there is a batch input, each batch has all 30,490 items included</t>
+  </si>
+  <si>
+    <t>1941 batch inputs (1 for each day) á (30,490; 7; 20)?</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,10 +676,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Changed Naming to version number, added V7 without any changes, just the copy to V6 as a starter
</commit_message>
<xml_diff>
--- a/src/models/Model_stats.xlsx
+++ b/src/models/Model_stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mf/Desktop/CS/Studies/7_Final_Project/Kaggle_M5PointPrediction/src/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393F79A5-A76F-F24A-A96E-581E01287723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CAA9EE-D9D3-6F43-9147-FB8431FDCF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{C69EC06E-22E8-864B-AAEF-80B6061A84A1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Modelle</t>
   </si>
@@ -150,6 +150,24 @@
   </si>
   <si>
     <t>Like V3 but only that a block of items get processed to check if V3 lacked of curse of dimensionality (like to process only the first 10 items and see what happens)</t>
+  </si>
+  <si>
+    <t>V6</t>
+  </si>
+  <si>
+    <t>Sliding window</t>
+  </si>
+  <si>
+    <t>1941, 7, feature_size</t>
+  </si>
+  <si>
+    <t>V7</t>
+  </si>
+  <si>
+    <t>Without sliding window</t>
+  </si>
+  <si>
+    <t>1, 1941, feature_size</t>
   </si>
 </sst>
 </file>
@@ -515,13 +533,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF780F6-B6D0-7C48-8B89-9537CB7819BD}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,6 +734,28 @@
       <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished Grid Search implementation in V8
</commit_message>
<xml_diff>
--- a/src/models/Model_stats.xlsx
+++ b/src/models/Model_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mf/Desktop/CS/Studies/7_Final_Project/Kaggle_M5PointPrediction/src/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CAA9EE-D9D3-6F43-9147-FB8431FDCF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FB40C9-E9ED-C948-A0D4-B1CFDAED6661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{C69EC06E-22E8-864B-AAEF-80B6061A84A1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Modelle</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>1, 1941, feature_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V8 </t>
+  </si>
+  <si>
+    <t>Like model 6 (V7 is deprecated and won't be used any more) but with grid search implemented</t>
   </si>
 </sst>
 </file>
@@ -533,13 +539,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF780F6-B6D0-7C48-8B89-9537CB7819BD}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,6 +763,14 @@
         <v>43</v>
       </c>
     </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
restructuring folder and v9 that loads final configuration from tuner runs
</commit_message>
<xml_diff>
--- a/src/models/Model_stats.xlsx
+++ b/src/models/Model_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mf/Desktop/CS/Studies/7_Final_Project/Kaggle_M5PointPrediction/src/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FB40C9-E9ED-C948-A0D4-B1CFDAED6661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5177680-64BE-0C48-879B-08D7E1C583D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{C69EC06E-22E8-864B-AAEF-80B6061A84A1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Modelle</t>
   </si>
@@ -164,9 +164,6 @@
     <t>V7</t>
   </si>
   <si>
-    <t>Without sliding window</t>
-  </si>
-  <si>
     <t>1, 1941, feature_size</t>
   </si>
   <si>
@@ -174,6 +171,15 @@
   </si>
   <si>
     <t>Like model 6 (V7 is deprecated and won't be used any more) but with grid search implemented</t>
+  </si>
+  <si>
+    <t>Without sliding window; deprecated, unsure how to build new model architecture</t>
+  </si>
+  <si>
+    <t>V9</t>
+  </si>
+  <si>
+    <t>Basically like model 6 but with abilty to read in config files</t>
   </si>
 </sst>
 </file>
@@ -539,13 +545,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF780F6-B6D0-7C48-8B89-9537CB7819BD}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,18 +763,26 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
         <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
-        <v>45</v>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjustment in imported statements in data preparation
</commit_message>
<xml_diff>
--- a/src/models/Model_stats.xlsx
+++ b/src/models/Model_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mf/Desktop/CS/Studies/7_Final_Project/Kaggle_M5PointPrediction/src/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5177680-64BE-0C48-879B-08D7E1C583D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB3C036-06AD-8B45-96F8-218A8C1CD44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{C69EC06E-22E8-864B-AAEF-80B6061A84A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C69EC06E-22E8-864B-AAEF-80B6061A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
   <si>
     <t>Modelle</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Adam</t>
   </si>
   <si>
-    <t>mse</t>
-  </si>
-  <si>
     <t>RMSE</t>
   </si>
   <si>
@@ -110,24 +107,12 @@
     <t>Result</t>
   </si>
   <si>
-    <t>Model didn't let me predict because it stated that the predicting shape is different from what was explicitly set in the input_shape parameter (althouth training (32,213430, 20) and predicting (27, 213430, 20) shape were the same</t>
-  </si>
-  <si>
-    <t>I didn't define</t>
-  </si>
-  <si>
-    <t>Model outputs only one time series with shape 27, 1. The predictions for sales_amount were completely off with only negative values although no negative sales_amounts were recorded. No clue where the rest of the predictions (30490 itmes) were.</t>
-  </si>
-  <si>
     <t>Result short</t>
   </si>
   <si>
     <t>negative</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Original model</t>
   </si>
   <si>
@@ -143,21 +128,9 @@
     <t>Zwischenstand - training hat sehr lang gedauert + komischerweise ist mit jedem Lauf die accuracy / metric um 1 besser geworden; In der Zwischenzeit hat Damian geschrieben und gesagt korrekt wäre die Architektur von V3, weswegen ich an dieser Stelle weitermache</t>
   </si>
   <si>
-    <t>1941 batch inputs (1 for each day) á (1; 7; 20*30,490) bzw. (1941, 7, ca. 20*30,490)</t>
-  </si>
-  <si>
-    <t>V3_group_items.ipynb</t>
-  </si>
-  <si>
-    <t>Like V3 but only that a block of items get processed to check if V3 lacked of curse of dimensionality (like to process only the first 10 items and see what happens)</t>
-  </si>
-  <si>
     <t>V6</t>
   </si>
   <si>
-    <t>Sliding window</t>
-  </si>
-  <si>
     <t>1941, 7, feature_size</t>
   </si>
   <si>
@@ -180,6 +153,76 @@
   </si>
   <si>
     <t>Basically like model 6 but with abilty to read in config files</t>
+  </si>
+  <si>
+    <t>Model didn't let me predict because it stated that the predicting shape is different from what was explicitly set in the input_shape parameter (althouth training (32,213430, 20) and predicting (27, 213430, 20) shape were the same; Model outputs only one time series with shape 27, 1. The predictions for sales_amount were completely off with only negative values although no negative sales_amounts were recorded. No clue where the rest of the predictions (30490 itmes) were.</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>Switched back from data generator to batch in one go</t>
+  </si>
+  <si>
+    <t>Like V3 but only that a block of items get processed to check if V3 lacked of curse of dimensionality (like to process only the first 10 items and see what happens); Stateful=True, Dropout layers</t>
+  </si>
+  <si>
+    <t>Sliding window; Tweedie loss function</t>
+  </si>
+  <si>
+    <t>Model architecture like V4, Implemented data pipeline</t>
+  </si>
+  <si>
+    <t>Short description</t>
+  </si>
+  <si>
+    <t>1 Bidirectional LSTM
+0-3 LSTM layers with respective dropout layers
+1 Self attention layer
+1 Global pooling
+1 Dense</t>
+  </si>
+  <si>
+    <t>Adam + lr scheduler</t>
+  </si>
+  <si>
+    <t>Tweedie</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>32, 64, 128, 256, 512</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>1941, 28, combination size, feature size</t>
+  </si>
+  <si>
+    <t>2 LSTM
+1 Dense</t>
+  </si>
+  <si>
+    <t>1 LSTM
+1 Dense</t>
+  </si>
+  <si>
+    <t>3 LSTM
+1 Dense</t>
+  </si>
+  <si>
+    <t>4-12</t>
+  </si>
+  <si>
+    <t>30 + early stopping</t>
   </si>
 </sst>
 </file>
@@ -223,14 +266,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,246 +604,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF780F6-B6D0-7C48-8B89-9537CB7819BD}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
-        <v>19</v>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="3" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="H3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3">
+      <c r="J3" s="5">
         <v>7</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="5">
         <v>32</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="5">
         <v>3</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="5">
+        <v>7</v>
+      </c>
+      <c r="K4" s="5">
+        <v>32</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>24</v>
+      <c r="B5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="5">
+        <v>7</v>
+      </c>
+      <c r="K5" s="5">
+        <v>32</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="str">
-        <f>D3</f>
-        <v>1 LSTM (50, tanh)
-1 Dense (1)</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" ref="E4:L4" si="0">E3</f>
-        <v>Adam</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>mse</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>RMSE</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v>(32, 213430, 20)</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>(32, 30490)</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
+    <row r="6" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="5">
+        <v>14</v>
+      </c>
+      <c r="K6" s="5">
         <v>32</v>
       </c>
-      <c r="L4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="L6" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="5">
+        <v>14</v>
+      </c>
+      <c r="K7" s="5">
+        <v>32</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="5">
         <v>28</v>
       </c>
-      <c r="N4" t="s">
-        <v>26</v>
+      <c r="K8" s="5">
+        <v>32</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="9" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="5">
+        <v>28</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="5">
+        <v>28</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" t="s">
-        <v>35</v>
+    <row r="11" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="5">
+        <v>28</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
-    </row>
+    <row r="12" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Final adjustments, commenting etc.
</commit_message>
<xml_diff>
--- a/src/models/Model_stats.xlsx
+++ b/src/models/Model_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mf/Desktop/CS/Studies/7_Final_Project/Kaggle_M5PointPrediction/src/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB3C036-06AD-8B45-96F8-218A8C1CD44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AD0C34-7956-364C-9A82-B1BFFA04F720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C69EC06E-22E8-864B-AAEF-80B6061A84A1}"/>
+    <workbookView xWindow="4800" yWindow="2300" windowWidth="28800" windowHeight="17500" xr2:uid="{C69EC06E-22E8-864B-AAEF-80B6061A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -143,9 +143,6 @@
     <t xml:space="preserve">V8 </t>
   </si>
   <si>
-    <t>Like model 6 (V7 is deprecated and won't be used any more) but with grid search implemented</t>
-  </si>
-  <si>
     <t>Without sliding window; deprecated, unsure how to build new model architecture</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>30 + early stopping</t>
+  </si>
+  <si>
+    <t>Like model 6 (V7 is deprecated and won't be used any more) but with keras tuner implemented</t>
   </si>
 </sst>
 </file>
@@ -246,12 +246,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -268,12 +274,8 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -284,10 +286,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -610,7 +614,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,417 +627,423 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="3">
+        <v>7</v>
+      </c>
+      <c r="K3" s="3">
+        <v>32</v>
+      </c>
+      <c r="L3" s="3">
+        <v>3</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3">
+        <v>7</v>
+      </c>
+      <c r="K4" s="3">
+        <v>32</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="3">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3">
+        <v>32</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="3">
+        <v>14</v>
+      </c>
+      <c r="K6" s="3">
+        <v>32</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="3">
+        <v>14</v>
+      </c>
+      <c r="K7" s="3">
+        <v>32</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="3">
+        <v>28</v>
+      </c>
+      <c r="K8" s="3">
+        <v>32</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>22</v>
+      <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="3">
+        <v>28</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="5" t="s">
+    <row r="10" spans="1:14" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="3">
+        <v>28</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="5">
-        <v>7</v>
-      </c>
-      <c r="K3" s="5">
-        <v>32</v>
-      </c>
-      <c r="L3" s="5">
-        <v>3</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>39</v>
+      <c r="L10" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="5" t="s">
+    <row r="11" spans="1:14" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" s="3">
+        <v>28</v>
+      </c>
+      <c r="K11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="5">
-        <v>7</v>
-      </c>
-      <c r="K4" s="5">
-        <v>32</v>
-      </c>
-      <c r="L4" s="8" t="s">
+      <c r="L11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="5">
-        <v>7</v>
-      </c>
-      <c r="K5" s="5">
-        <v>32</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="5">
-        <v>14</v>
-      </c>
-      <c r="K6" s="5">
-        <v>32</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="5">
-        <v>14</v>
-      </c>
-      <c r="K7" s="5">
-        <v>32</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J8" s="5">
-        <v>28</v>
-      </c>
-      <c r="K8" s="5">
-        <v>32</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" s="5">
-        <v>28</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J10" s="5">
-        <v>28</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J11" s="5">
-        <v>28</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:14" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>